<commit_message>
XZ YZ plots and first motion picks
</commit_message>
<xml_diff>
--- a/fallClean/RaceInfo/fa_info_sat.xlsx
+++ b/fallClean/RaceInfo/fa_info_sat.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Desktop/dragraceAnalysis-master/fallClean/RaceInfo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Library/Containers/com.microsoft.Excel/Data/Desktop/dragraceAnalysis-master/fallClean/RaceInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79A213F-AF74-8144-ACD2-02435B689650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A586D6EC-6155-D34D-B5AE-B5AC1DAD1DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="13820" xr2:uid="{9DCAC0C9-DACB-1A4F-8007-B7FE5A0F0F7F}"/>
+    <workbookView xWindow="12620" yWindow="2960" windowWidth="15800" windowHeight="13820" xr2:uid="{9DCAC0C9-DACB-1A4F-8007-B7FE5A0F0F7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451A4CC6-0841-1048-BD58-20CC18F60859}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127:D129"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>